<commit_message>
update main run script
</commit_message>
<xml_diff>
--- a/peraja09_financial_forecasting.xlsx
+++ b/peraja09_financial_forecasting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuransun/Desktop/project/q1/q1-financial-health-analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACB29CE3-4539-FF4C-93DA-85520A389A3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9DFDEC8-E9F1-A344-8352-72217EC47167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4320" yWindow="500" windowWidth="34080" windowHeight="19340" xr2:uid="{5FD120CE-189A-7142-A9BC-9DF14CA740FA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="230">
   <si>
     <t>module 1: operating activities</t>
   </si>
@@ -654,9 +654,6 @@
     <t>then calculate cash budget at year 1, and loan schedule at year 1</t>
   </si>
   <si>
-    <t>the computation order is after calculating cash budget and loan schedule at year 0</t>
-  </si>
-  <si>
     <t>intermedia tables are calculated before the following iterative IS-CB calculation</t>
   </si>
   <si>
@@ -724,6 +721,12 @@
   </si>
   <si>
     <t xml:space="preserve">advance payment from customers -&gt; liability. Receive cash, but not actually give them products. </t>
+  </si>
+  <si>
+    <t>finally use all the above results to construct balance sheet</t>
+  </si>
+  <si>
+    <t>the computation order is after calculating cash budget,  loan schedule and income statement at year 0</t>
   </si>
 </sst>
 </file>
@@ -1268,10 +1271,10 @@
   <dimension ref="A2:M266"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C228" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="K5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="J252" sqref="J252"/>
+      <selection pane="bottomRight" activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1651,7 +1654,7 @@
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
       <c r="M27" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
@@ -1666,7 +1669,7 @@
       <c r="G28" s="8"/>
       <c r="H28" s="8"/>
       <c r="M28" t="s">
-        <v>205</v>
+        <v>229</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
@@ -1717,7 +1720,7 @@
       <c r="G31" s="8"/>
       <c r="H31" s="8"/>
       <c r="M31" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
@@ -1732,7 +1735,7 @@
       <c r="G32" s="8"/>
       <c r="H32" s="8"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>39</v>
       </c>
@@ -1743,8 +1746,11 @@
       <c r="F33" s="8"/>
       <c r="G33" s="8"/>
       <c r="H33" s="8"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M33" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>40</v>
       </c>
@@ -1756,7 +1762,7 @@
       <c r="G34" s="8"/>
       <c r="H34" s="8"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>41</v>
       </c>
@@ -1768,7 +1774,7 @@
       <c r="G35" s="8"/>
       <c r="H35" s="8"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>42</v>
       </c>
@@ -1780,7 +1786,7 @@
       <c r="G36" s="8"/>
       <c r="H36" s="8"/>
     </row>
-    <row r="37" spans="1:8" ht="46" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" ht="46" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="10" t="s">
         <v>43</v>
       </c>
@@ -1792,7 +1798,7 @@
       <c r="G37" s="8"/>
       <c r="H37" s="8"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>44</v>
       </c>
@@ -1804,7 +1810,7 @@
       <c r="G38" s="8"/>
       <c r="H38" s="8"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>45</v>
       </c>
@@ -1822,7 +1828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>46</v>
       </c>
@@ -1834,7 +1840,7 @@
       </c>
       <c r="H40" s="6"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>48</v>
       </c>
@@ -1845,7 +1851,7 @@
       <c r="G41" s="6"/>
       <c r="H41" s="6"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>49</v>
       </c>
@@ -1860,7 +1866,7 @@
       </c>
       <c r="H42" s="6"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>57</v>
       </c>
@@ -1870,7 +1876,7 @@
       <c r="G45" s="6"/>
       <c r="H45" s="6"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>50</v>
       </c>
@@ -1892,7 +1898,7 @@
         <v>6.0499999999999998E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>51</v>
       </c>
@@ -1914,7 +1920,7 @@
         <v>6.0499999999999998E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>52</v>
       </c>
@@ -2285,7 +2291,7 @@
         <v>0</v>
       </c>
       <c r="J70" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.2">
@@ -2393,7 +2399,7 @@
         <v>4.4315551400144999</v>
       </c>
       <c r="J77" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.2">
@@ -2477,7 +2483,7 @@
         <v>26.015666688976079</v>
       </c>
       <c r="J83" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.2">
@@ -2734,7 +2740,7 @@
         <v>23.993357584135634</v>
       </c>
       <c r="J99" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.2">
@@ -2788,7 +2794,7 @@
         <v>407.88707893030573</v>
       </c>
       <c r="J101" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.2">
@@ -2920,7 +2926,7 @@
         <v>22.180951996501495</v>
       </c>
       <c r="J110" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.2">
@@ -2948,7 +2954,7 @@
         <v>0</v>
       </c>
       <c r="J111" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.2">
@@ -2976,7 +2982,7 @@
         <v>407.88707893030573</v>
       </c>
       <c r="J112" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.2">
@@ -3247,7 +3253,7 @@
         <v>8.655488191238371</v>
       </c>
       <c r="J130" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.2">
@@ -3383,7 +3389,7 @@
         <v>1</v>
       </c>
       <c r="J143" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.2">
@@ -3411,7 +3417,7 @@
         <v>0</v>
       </c>
       <c r="J144" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.2">
@@ -3439,7 +3445,7 @@
         <v>10.998394061860756</v>
       </c>
       <c r="J145" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="146" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3704,7 +3710,7 @@
         <v>10.892965391041301</v>
       </c>
       <c r="J161" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="162" spans="1:10" x14ac:dyDescent="0.2">
@@ -3732,7 +3738,7 @@
         <v>0</v>
       </c>
       <c r="J162" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="164" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -3793,7 +3799,7 @@
         <v>0</v>
       </c>
       <c r="J169" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.2">
@@ -4631,7 +4637,7 @@
         <v>0</v>
       </c>
       <c r="J226" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="227" spans="1:10" x14ac:dyDescent="0.2">
@@ -4758,7 +4764,7 @@
         <v>11.252134648609882</v>
       </c>
       <c r="J232" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="233" spans="1:10" x14ac:dyDescent="0.2">
@@ -4787,7 +4793,7 @@
         <v>12.086845555403535</v>
       </c>
       <c r="J233" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="237" spans="1:10" x14ac:dyDescent="0.2">
@@ -4906,7 +4912,7 @@
         <v>0</v>
       </c>
       <c r="J242" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="243" spans="1:10" x14ac:dyDescent="0.2">
@@ -4935,7 +4941,7 @@
         <v>0</v>
       </c>
       <c r="J243" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="244" spans="1:10" x14ac:dyDescent="0.2">
@@ -5089,7 +5095,7 @@
         <v>0</v>
       </c>
       <c r="J251" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="252" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
update yfinance data fetch script
</commit_message>
<xml_diff>
--- a/peraja09_financial_forecasting.xlsx
+++ b/peraja09_financial_forecasting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuransun/Desktop/project/q1/q1-financial-health-analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9DFDEC8-E9F1-A344-8352-72217EC47167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F142C7-DA57-4C42-B441-B335637A8C14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4320" yWindow="500" windowWidth="34080" windowHeight="19340" xr2:uid="{5FD120CE-189A-7142-A9BC-9DF14CA740FA}"/>
   </bookViews>
@@ -705,18 +705,12 @@
     <t>pay last year's dividens, year +1</t>
   </si>
   <si>
-    <t>lat year ending balance loan * norminal interest rate this year (real interest rate is fixed)</t>
-  </si>
-  <si>
     <t>cumulated earnings of all previous years</t>
   </si>
   <si>
     <t>record in next year. Here is only a calculation to show how much will be paid.</t>
   </si>
   <si>
-    <t>payment to supplier-&gt;asset, can regard as using cash to buy future assets</t>
-  </si>
-  <si>
     <t>from cash budget</t>
   </si>
   <si>
@@ -727,6 +721,12 @@
   </si>
   <si>
     <t>the computation order is after calculating cash budget,  loan schedule and income statement at year 0</t>
+  </si>
+  <si>
+    <t>last year ending balance loan * norminal interest rate this year (real interest rate is fixed)</t>
+  </si>
+  <si>
+    <t>advance payment to supplier-&gt;asset, can regard as using cash to buy future assets</t>
   </si>
 </sst>
 </file>
@@ -1271,10 +1271,10 @@
   <dimension ref="A2:M266"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="K5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C121" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="M29" sqref="M29"/>
+      <selection pane="bottomRight" activeCell="J242" sqref="J242"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1669,7 +1669,7 @@
       <c r="G28" s="8"/>
       <c r="H28" s="8"/>
       <c r="M28" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
@@ -1747,7 +1747,7 @@
       <c r="G33" s="8"/>
       <c r="H33" s="8"/>
       <c r="M33" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
@@ -4637,7 +4637,7 @@
         <v>0</v>
       </c>
       <c r="J226" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
     </row>
     <row r="227" spans="1:10" x14ac:dyDescent="0.2">
@@ -4764,7 +4764,7 @@
         <v>11.252134648609882</v>
       </c>
       <c r="J232" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="233" spans="1:10" x14ac:dyDescent="0.2">
@@ -4793,7 +4793,7 @@
         <v>12.086845555403535</v>
       </c>
       <c r="J233" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="237" spans="1:10" x14ac:dyDescent="0.2">
@@ -4912,7 +4912,7 @@
         <v>0</v>
       </c>
       <c r="J242" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
     </row>
     <row r="243" spans="1:10" x14ac:dyDescent="0.2">
@@ -4941,7 +4941,7 @@
         <v>0</v>
       </c>
       <c r="J243" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="244" spans="1:10" x14ac:dyDescent="0.2">
@@ -5095,7 +5095,7 @@
         <v>0</v>
       </c>
       <c r="J251" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="252" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>